<commit_message>
Seemed to have fixed random null values in distributors xl
</commit_message>
<xml_diff>
--- a/server/resources/Distributors.xlsx
+++ b/server/resources/Distributors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylelevy/code/nextjs-code-challenge/server/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Documents\[Coding Projects]\topbloc-code-challenge\server\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50C8CE1-2C4A-E547-90D0-FB5945BB241A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FEDD11-E0A2-4190-AC32-429859FCCB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="18700" activeTab="2" xr2:uid="{55F9AAF4-5023-6A4C-B2E9-1E49E110F345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{55F9AAF4-5023-6A4C-B2E9-1E49E110F345}"/>
   </bookViews>
   <sheets>
     <sheet name="Candy Corp" sheetId="1" r:id="rId1"/>
@@ -458,18 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5DF09A-8712-0349-8B63-36BB778FDA93}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +480,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -502,7 +502,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -513,7 +513,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -524,23 +524,9 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -552,12 +538,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -579,7 +565,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -590,7 +576,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -601,7 +587,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -612,7 +598,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -623,7 +609,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -634,7 +620,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -645,7 +631,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -656,7 +642,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -667,7 +653,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -678,7 +664,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -689,7 +675,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -700,7 +686,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -711,7 +697,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -722,7 +708,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -742,16 +728,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E13DAFF-8F71-B54E-92DC-3370EFEE3E1C}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -762,7 +748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -773,7 +759,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -784,7 +770,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -795,7 +781,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -806,7 +792,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -817,7 +803,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -828,7 +814,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -839,7 +825,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>

</xml_diff>